<commit_message>
Export database again to make sure everything is up to date
</commit_message>
<xml_diff>
--- a/resources/pomXml.xlsx
+++ b/resources/pomXml.xlsx
@@ -561,7 +561,7 @@
       </c>
       <c r="Z1" s="1" t="inlineStr">
         <is>
-          <t>GoogleCloudFilestore</t>
+          <t>GoogleCloudFirestore</t>
         </is>
       </c>
       <c r="AA1" s="1" t="inlineStr">
@@ -4893,7 +4893,7 @@
         <v>0</v>
       </c>
       <c r="J24" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="K24" t="n">
         <v>0</v>
@@ -6018,10 +6018,8 @@
       <c r="I30" t="n">
         <v>0</v>
       </c>
-      <c r="J30" t="inlineStr">
-        <is>
-          <t>contrib/storage-jdbc/pom.xml</t>
-        </is>
+      <c r="J30" t="n">
+        <v>0</v>
       </c>
       <c r="K30" t="n">
         <v>0</v>
@@ -6147,10 +6145,8 @@
           <t>metastore/rdbms-metastore/README.md</t>
         </is>
       </c>
-      <c r="AW30" t="inlineStr">
-        <is>
-          <t>contrib/storage-jdbc/pom.xml</t>
-        </is>
+      <c r="AW30" t="n">
+        <v>0</v>
       </c>
       <c r="AX30" t="inlineStr">
         <is>
@@ -9443,7 +9439,7 @@
         <v>0</v>
       </c>
       <c r="J48" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="K48" t="n">
         <v>0</v>
@@ -19762,7 +19758,7 @@
         <v>0</v>
       </c>
       <c r="J103" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="K103" t="n">
         <v>0</v>
@@ -24640,7 +24636,7 @@
         <v>0</v>
       </c>
       <c r="J129" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="K129" t="n">
         <v>0</v>
@@ -24763,7 +24759,7 @@
         <v>10</v>
       </c>
       <c r="AW129" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="AX129" t="n">
         <v>0</v>
@@ -25207,7 +25203,7 @@
         <v>0</v>
       </c>
       <c r="J132" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K132" t="n">
         <v>0</v>
@@ -25330,7 +25326,7 @@
         <v>2</v>
       </c>
       <c r="AW132" t="n">
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="AX132" t="n">
         <v>-1</v>
@@ -25784,7 +25780,7 @@
         <v>0</v>
       </c>
       <c r="J135" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K135" t="n">
         <v>0</v>
@@ -25903,7 +25899,7 @@
         <v>3</v>
       </c>
       <c r="AW135" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AX135" t="n">
         <v>0</v>
@@ -31967,7 +31963,7 @@
         <v>0</v>
       </c>
       <c r="J168" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K168" t="n">
         <v>0</v>
@@ -32084,7 +32080,7 @@
         <v>2</v>
       </c>
       <c r="AW168" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AX168" t="n">
         <v>0</v>
@@ -50578,7 +50574,7 @@
         <v>0</v>
       </c>
       <c r="J267" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="K267" t="n">
         <v>0</v>
@@ -61071,10 +61067,8 @@
       <c r="I323" t="n">
         <v>0</v>
       </c>
-      <c r="J323" t="inlineStr">
-        <is>
-          <t>spring-batch-core/pom.xml</t>
-        </is>
+      <c r="J323" t="n">
+        <v>0</v>
       </c>
       <c r="K323" t="n">
         <v>0</v>
@@ -61200,10 +61194,8 @@
           <t>spring-batch-core/src/test/java/org/springframework/batch/core/test/repository/PostgreSQLJobRepositoryIntegrationTests.java</t>
         </is>
       </c>
-      <c r="AW323" t="inlineStr">
-        <is>
-          <t>spring-batch-core/pom.xml</t>
-        </is>
+      <c r="AW323" t="n">
+        <v>0</v>
       </c>
       <c r="AX323" t="n">
         <v>0</v>
@@ -67278,10 +67270,8 @@
       <c r="I356" t="n">
         <v>0</v>
       </c>
-      <c r="J356" t="inlineStr">
-        <is>
-          <t>testsuite/pom.xml</t>
-        </is>
+      <c r="J356" t="n">
+        <v>0</v>
       </c>
       <c r="K356" t="n">
         <v>0</v>
@@ -68606,7 +68596,7 @@
         <v>0</v>
       </c>
       <c r="J363" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="K363" t="n">
         <v>0</v>

</xml_diff>